<commit_message>
Add real PDF thumbnail preview functionality with PDF.js integration
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/final_invoice_data.xlsx
+++ b/process/outputs/excel_files/final_invoice_data.xlsx
@@ -600,22 +600,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>4852929</t>
+          <t>48529.29</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>441685</t>
+          <t>4416.85</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>102125</t>
+          <t>1021.25</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>4309119</t>
+          <t>43091.19</t>
         </is>
       </c>
       <c r="M2" t="n">
@@ -636,7 +636,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>captive aire_1754662125633.pdf</t>
+          <t>captive aire_1754689853322.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Complete invoice processing redesign: Added preview buttons to approval dialogs, redesigned Processed Invoices section with thumbnails and full-screen modal, implemented automatic file preservation, fixed scrolling issues, and updated Batch_Code to use today's date
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/final_invoice_data.xlsx
+++ b/process/outputs/excel_files/final_invoice_data.xlsx
@@ -437,7 +437,7 @@
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="36" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
@@ -452,7 +452,7 @@
     <col width="12" customWidth="1" min="17" max="17"/>
     <col width="11" customWidth="1" min="18" max="18"/>
     <col width="9" customWidth="1" min="19" max="19"/>
-    <col width="32" customWidth="1" min="20" max="20"/>
+    <col width="30" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -560,27 +560,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TST</t>
+          <t>AA1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>08/04/25</t>
+          <t>08/07/25</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>testraj</t>
+          <t>2025-08-14</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CAPAIR</t>
+          <t>NORWRI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Captive Aire</t>
+          <t>Norman S. Wright Mech. Equip. LLC.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -590,53 +590,48 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2457243</t>
+          <t>127310</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>08/04/25</t>
+          <t>08/07/25</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>48529.29</t>
+          <t>74143.65</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>4416.85</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>1021.25</t>
+          <t>6663.65</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>43091.19</t>
+          <t>67480.00</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>5030</t>
+          <t>5040</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>captive aire_1754943103394.pdf</t>
+          <t>127310 nsw_1755208409430.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add network configuration for Project List file access and update invoice pipeline
</commit_message>
<xml_diff>
--- a/process/outputs/excel_files/final_invoice_data.xlsx
+++ b/process/outputs/excel_files/final_invoice_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,7 +437,7 @@
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="27" customWidth="1" min="5" max="5"/>
+    <col width="36" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
     <col width="16" customWidth="1" min="7" max="7"/>
     <col width="14" customWidth="1" min="8" max="8"/>
@@ -565,7 +565,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>08/21/25</t>
+          <t>08/13/25</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -575,12 +575,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RSDTOT</t>
+          <t>NORWRI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RSD</t>
+          <t>Norman S. Wright Mech. Equip. LLC.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -590,48 +590,48 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>11395918-00</t>
+          <t>127813</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>08/21/25</t>
+          <t>08/13/25</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>186.74</t>
+          <t>821.02</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>18.13</t>
+          <t>73.79</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>168.61</t>
-        </is>
-      </c>
-      <c r="N2" t="n">
-        <v>25.19</v>
+          <t>747.23</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>1466</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>5030</t>
+          <t>5040</t>
         </is>
       </c>
       <c r="Q2" t="n">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>E</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>1_1755887243708.pdf</t>
+          <t>127813_1755894601049.pdf</t>
         </is>
       </c>
     </row>
@@ -668,7 +668,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>39395877-00</t>
+          <t>11395918-00</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -678,21 +678,21 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>324.04</t>
+          <t>186.74</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>29.13</t>
+          <t>18.13</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>294.91</t>
+          <t>168.61</t>
         </is>
       </c>
       <c r="N3" t="n">
-        <v>25.16</v>
+        <v>25.19</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>2_1755887243712.pdf</t>
+          <t>1_1755894595697.pdf</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>39395879-00</t>
+          <t>39395877-00</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -756,21 +756,21 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>997.32</t>
+          <t>324.04</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>89.64</t>
+          <t>29.13</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>907.68</t>
+          <t>294.91</t>
         </is>
       </c>
       <c r="N4" t="n">
-        <v>24.68</v>
+        <v>25.16</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>3_1755887243715.pdf</t>
+          <t>2_1755894595700.pdf</t>
         </is>
       </c>
     </row>
@@ -809,12 +809,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>JONSUP</t>
+          <t>RSDTOT</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Johnstone Supply</t>
+          <t>RSD</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>101130827.1</t>
+          <t>39395879-00</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -834,35 +834,38 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>783.30</t>
+          <t>997.32</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>70.40</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0.00</t>
+          <t>89.64</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>712.90</t>
-        </is>
-      </c>
-      <c r="O5" t="n">
-        <v>13616</v>
+          <t>907.68</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>24.68</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>5260</t>
+          <t>5030</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>320</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>4_1755887243717.pdf</t>
+          <t>3_1755894595693.pdf</t>
         </is>
       </c>
     </row>
@@ -884,12 +887,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>LORSON</t>
+          <t>JONSUP</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Lord &amp; Sons Inc.</t>
+          <t>Johnstone Supply</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -897,6 +900,11 @@
           <t>I</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>101130827.1</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>08/21/25</t>
@@ -904,12 +912,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>31.31</t>
+          <t>783.30</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>2.81</t>
+          <t>70.40</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -919,22 +927,20 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>28.50</t>
-        </is>
+          <t>712.90</t>
+        </is>
+      </c>
+      <c r="O6" t="n">
+        <v>13616</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>SHOP STOCK</t>
+          <t>5260</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>inv-01-875854.pdf_page_1_1755887243721.pdf</t>
+          <t>4_1755894595691.pdf</t>
         </is>
       </c>
     </row>
@@ -956,68 +962,140 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>LORSON</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Lord &amp; Sons Inc.</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>08/21/25</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>31.31</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>2.81</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>28.50</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>SHOP STOCK</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>inv-01-875854.pdf_page_1_1755894595704.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AA1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>08/21/25</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-08-22</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>CALHYD</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>California Hydronics Corp</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>SIN221250</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>08/21/25</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>377.97</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>33.97</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>0.00</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>344.00</t>
         </is>
       </c>
-      <c r="M7" t="n">
+      <c r="M8" t="n">
         <v>1504</v>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="P8" t="inlineStr">
         <is>
           <t>5030</t>
         </is>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q8" t="n">
         <v>320</v>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="R8" t="inlineStr">
         <is>
           <t>M</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>sin221250_page_1_1755887243722.pdf</t>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>sin221250_page_1_1755894595706.pdf</t>
         </is>
       </c>
     </row>

</xml_diff>